<commit_message>
Updated with our data
</commit_message>
<xml_diff>
--- a/data_files/output/clustering/bestK.xlsx
+++ b/data_files/output/clustering/bestK.xlsx
@@ -396,7 +396,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -404,7 +404,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>